<commit_message>
Empty rows removed from Excel
</commit_message>
<xml_diff>
--- a/test_files/601_Extensions.xlsx
+++ b/test_files/601_Extensions.xlsx
@@ -59,17 +59,13 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="3">
+  <fonts count="2">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
   </fonts>
@@ -87,15 +83,12 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+      <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -158,8 +151,8 @@
       <c r="E2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
@@ -177,44 +170,8 @@
       <c r="E3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-    </row>
-    <row r="4">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-    </row>
-    <row r="5">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-    </row>
-    <row r="6">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-    </row>
-    <row r="7">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>